<commit_message>
avances en descargar excel
</commit_message>
<xml_diff>
--- a/apps/templates/EXCEL/remisiones.xlsx
+++ b/apps/templates/EXCEL/remisiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\templates\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C29377C-2D40-4B81-A5B9-D2425BE0739A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA092C88-826D-444F-B597-99096565FF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BFB0A6B-61D2-4748-9625-7D939A6F5CCD}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>a</t>
   </si>
@@ -116,30 +116,18 @@
     <t>CLIENTE</t>
   </si>
   <si>
-    <t>ANDRES OTALORA S.A.S</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
-    <t>30/ago/2024</t>
-  </si>
-  <si>
     <t>DIRECCIÓN</t>
   </si>
   <si>
-    <t>AV 6 BIS 27 N 24 BRR SANTA MONICA</t>
-  </si>
-  <si>
     <t>TELEFONO</t>
   </si>
   <si>
     <t>CIUDAD</t>
   </si>
   <si>
-    <t>CALI</t>
-  </si>
-  <si>
     <t>OC</t>
   </si>
   <si>
@@ -149,9 +137,6 @@
     <t>DESTINATARIO</t>
   </si>
   <si>
-    <t>LINA</t>
-  </si>
-  <si>
     <t>REMISIÓN #</t>
   </si>
   <si>
@@ -173,12 +158,6 @@
     <t>SALDO DE DESPACHO</t>
   </si>
   <si>
-    <t>REF.INTERNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SALDO_DEPACHO</t>
-  </si>
-  <si>
     <t>LEANDRO ESCARRIA</t>
   </si>
   <si>
@@ -186,6 +165,9 @@
   </si>
   <si>
     <t>RECIBE:</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -194,14 +176,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -248,6 +222,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -257,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -376,17 +358,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -414,9 +385,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -434,30 +405,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -467,122 +426,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -912,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9F5A1-4611-4F3F-A852-7E08544F7F8D}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:G53"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,11 +854,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
@@ -941,11 +867,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -954,108 +880,108 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="B5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="G5" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="14">
-        <v>3173534798</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="G6" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B7" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2407</v>
+      <c r="G7" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1063,8 +989,8 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1072,8 +998,8 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1081,8 +1007,8 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1090,8 +1016,8 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1102,8 +1028,8 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1114,8 +1040,8 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1126,8 +1052,8 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1138,8 +1064,8 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1150,8 +1076,8 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1162,8 +1088,8 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1174,8 +1100,8 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1186,8 +1112,8 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1198,8 +1124,8 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1210,8 +1136,8 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1222,8 +1148,8 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1234,8 +1160,8 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1246,8 +1172,8 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1258,8 +1184,8 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1270,8 +1196,8 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1282,8 +1208,8 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1291,8 +1217,8 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1300,8 +1226,8 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1309,8 +1235,8 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1318,8 +1244,8 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1327,8 +1253,8 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1336,211 +1262,193 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="36">
         <f>SUM(F10:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="34"/>
+      <c r="G36" s="37"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="8" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="19"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="37"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="40"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="40"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="40"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="40"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="38"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="40"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="38"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="40"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="38"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="40"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="38"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="40"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="40"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="38"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="40"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="38"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="43"/>
+      <c r="B53" s="13"/>
+      <c r="D53" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="B54" s="13"/>
       <c r="D54" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="D55" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B55" s="13"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="17"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="17"/>
+      <c r="B56" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A39:G53"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+  <mergeCells count="28">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
@@ -1553,19 +1461,16 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A38:G52"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
se añade modal para registrar persona que recibe remisión
</commit_message>
<xml_diff>
--- a/apps/templates/EXCEL/remisiones.xlsx
+++ b/apps/templates/EXCEL/remisiones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\templates\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA092C88-826D-444F-B597-99096565FF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1834426-FE87-4C6A-A5F2-A5DE17C98C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BFB0A6B-61D2-4748-9625-7D939A6F5CCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3BFB0A6B-61D2-4748-9625-7D939A6F5CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>a</t>
   </si>
@@ -131,9 +131,6 @@
     <t>OC</t>
   </si>
   <si>
-    <t>ANDRES OTALORA</t>
-  </si>
-  <si>
     <t>DESTINATARIO</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
   </si>
   <si>
     <t>SALDO DE DESPACHO</t>
-  </si>
-  <si>
-    <t>LEANDRO ESCARRIA</t>
   </si>
   <si>
     <t>ENTREGA:</t>
@@ -426,6 +420,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -453,56 +492,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,25 +834,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9F5A1-4611-4F3F-A852-7E08544F7F8D}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2"/>
-    <col min="2" max="3" width="25.7109375" style="2" customWidth="1"/>
-    <col min="4" max="6" width="20.7109375" style="2"/>
-    <col min="7" max="7" width="26.140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="20.7109375" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2"/>
+    <col min="2" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="2"/>
+    <col min="5" max="5" width="23.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="20.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+    <row r="1" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
@@ -866,12 +862,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+    <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -879,145 +875,145 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="B4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+      <c r="B5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="B6" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1026,10 +1022,10 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1038,10 +1034,10 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1050,7 +1046,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
@@ -1062,7 +1058,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -1074,7 +1070,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -1086,7 +1082,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
@@ -1098,7 +1094,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -1110,7 +1106,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -1122,10 +1118,10 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1134,10 +1130,10 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1146,10 +1142,10 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1158,10 +1154,10 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1170,10 +1166,10 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1182,10 +1178,10 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1194,10 +1190,10 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1206,73 +1202,73 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="36">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="38">
         <f>SUM(F10:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="37"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="39"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1281,174 +1277,175 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="19"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="19"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="19"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="19"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="19"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="19"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="19"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="29"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="31"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="32"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="34"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="32"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="34"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="34"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="34"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="34"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="34"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="34"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="32"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="34"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="35"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="37"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="D53" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="13"/>
-      <c r="D54" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="13"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A38:G52"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
@@ -1461,15 +1458,13 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A38:G52"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
se agrega saldo pendiente en observaciones de la remision
</commit_message>
<xml_diff>
--- a/apps/templates/EXCEL/remisiones.xlsx
+++ b/apps/templates/EXCEL/remisiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\templates\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1834426-FE87-4C6A-A5F2-A5DE17C98C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419B783E-BF94-4C3E-9F71-41A27B23F3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3BFB0A6B-61D2-4748-9625-7D939A6F5CCD}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>a</t>
   </si>
@@ -426,6 +426,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,59 +465,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9F5A1-4611-4F3F-A852-7E08544F7F8D}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,11 +850,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
@@ -863,11 +863,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -884,12 +884,12 @@
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -901,12 +901,12 @@
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
@@ -918,12 +918,12 @@
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
@@ -935,12 +935,12 @@
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
@@ -957,10 +957,10 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
@@ -976,8 +976,8 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -985,8 +985,8 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -994,8 +994,8 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1003,8 +1003,8 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1012,8 +1012,8 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1024,8 +1024,8 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1036,8 +1036,8 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1120,8 +1120,8 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1132,8 +1132,8 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1144,8 +1144,8 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1156,8 +1156,8 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1168,8 +1168,8 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1180,8 +1180,8 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1192,8 +1192,8 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1204,8 +1204,8 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1213,8 +1213,8 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1222,8 +1222,8 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1231,8 +1231,8 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1240,8 +1240,8 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1249,8 +1249,8 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1262,11 +1262,11 @@
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="38">
+      <c r="F36" s="17">
         <f>SUM(F10:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="39"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
@@ -1278,139 +1278,141 @@
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="31"/>
+      <c r="A38" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="32"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="34"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="32"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="32"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="34"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="34"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="34"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="32"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="34"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="32"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="35"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="37"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="39"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" s="13"/>
@@ -1437,15 +1439,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A38:G52"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
@@ -1458,13 +1458,15 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A38:G52"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>